<commit_message>
added in chaining of linear regression models to predict game scores
</commit_message>
<xml_diff>
--- a/ANN Lifetime Predictions.xlsx
+++ b/ANN Lifetime Predictions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thigg\Desktop\Hockey Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255AEBE7-0759-4B59-9013-2FEA9572B000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6BC553-56D2-4D1A-99D5-7DB330BBEA1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pivot" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="3" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>Date</t>
   </si>
@@ -197,6 +197,9 @@
   </si>
   <si>
     <t>Playing At:  Pittsburgh Penguins   Home</t>
+  </si>
+  <si>
+    <t>50-60</t>
   </si>
 </sst>
 </file>
@@ -681,7 +684,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -690,6 +693,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -750,25 +754,25 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Thomas Higgins" refreshedDate="45278.317295370369" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="72" xr:uid="{00000000-000A-0000-FFFF-FFFF11000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Thomas Higgins" refreshedDate="45278.947084027779" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="72" xr:uid="{00000000-000A-0000-FFFF-FFFF11000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:H1048576" sheet="Predictions"/>
   </cacheSource>
   <cacheFields count="9">
     <cacheField name="Date" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-17T00:00:00" maxDate="2023-12-18T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2023-12-17T00:00:00" maxDate="2023-12-19T00:00:00"/>
     </cacheField>
     <cacheField name="Winner" numFmtId="0">
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Winner Probability" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.60019999999999996" maxValue="0.77388000000000001"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.55600000000000005" maxValue="0.77388000000000001"/>
     </cacheField>
     <cacheField name="Loser" numFmtId="0">
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Loser Probability" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.22611999999999999" maxValue="0.39979999999999999"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.22611999999999999" maxValue="0.44400000000000001"/>
     </cacheField>
     <cacheField name="Site" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -780,10 +784,10 @@
       <sharedItems containsBlank="1" count="7">
         <s v="70-80"/>
         <s v="60-70"/>
+        <s v="50-60"/>
         <m/>
         <s v="85 &lt;" u="1"/>
         <s v="80-85" u="1"/>
-        <s v="50-60" u="1"/>
         <s v="&gt; 85" u="1"/>
       </sharedItems>
     </cacheField>
@@ -850,23 +854,53 @@
     <x v="1"/>
   </r>
   <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
+    <d v="2023-12-18T00:00:00"/>
+    <s v="Winnipeg Jets"/>
+    <n v="0.70899999999999996"/>
+    <s v="Montreal Canadiens"/>
+    <n v="0.29099999999999998"/>
+    <s v="Playing At:  Winnipeg Jets   Home"/>
+    <n v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <d v="2023-12-18T00:00:00"/>
+    <s v="Dallas Stars"/>
+    <n v="0.66300000000000003"/>
+    <s v="Seattle Kraken"/>
+    <n v="0.33700000000000002"/>
+    <s v="Playing At:  Dallas Stars   Home"/>
+    <n v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2023-12-18T00:00:00"/>
+    <s v="Detroit Red Wings"/>
+    <n v="0.65200000000000002"/>
+    <s v="Anaheim Ducks"/>
+    <n v="0.34799999999999998"/>
+    <s v="Playing At:  Detroit Red Wings   Home"/>
+    <n v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <d v="2023-12-18T00:00:00"/>
+    <s v="Florida Panthers"/>
+    <n v="0.58099999999999996"/>
+    <s v="Calgary Flames"/>
+    <n v="0.41899999999999998"/>
+    <s v="Playing At:  Calgary Flames   Home"/>
+    <n v="1"/>
     <x v="2"/>
   </r>
   <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
+    <d v="2023-12-18T00:00:00"/>
+    <s v="Pittsburgh Penguins"/>
+    <n v="0.55600000000000005"/>
+    <s v="Minnesota Wild"/>
+    <n v="0.44400000000000001"/>
+    <s v="Playing At:  Pittsburgh Penguins   Home"/>
+    <n v="1"/>
     <x v="2"/>
   </r>
   <r>
@@ -877,654 +911,624 @@
     <m/>
     <m/>
     <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <x v="2"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="3"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:C6" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:C7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
     <pivotField dataField="1" showAll="0"/>
@@ -1535,12 +1539,12 @@
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisRow" showAll="0" sortType="descending">
       <items count="8">
-        <item h="1" x="2"/>
-        <item m="1" x="3"/>
+        <item h="1" x="3"/>
         <item m="1" x="4"/>
+        <item m="1" x="5"/>
         <item x="0"/>
         <item x="1"/>
-        <item m="1" x="5"/>
+        <item x="2"/>
         <item h="1" m="1" x="6"/>
         <item t="default"/>
       </items>
@@ -1550,12 +1554,15 @@
   <rowFields count="1">
     <field x="7"/>
   </rowFields>
-  <rowItems count="3">
+  <rowItems count="4">
     <i>
       <x v="3"/>
     </i>
     <i>
       <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
     </i>
     <i t="grand">
       <x/>
@@ -1887,20 +1894,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -1917,34 +1924,34 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="6">
+        <v>2</v>
+      </c>
+      <c r="C4" s="6">
         <v>1</v>
       </c>
       <c r="D4" s="5">
         <f>C4/B4</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F4">
         <f>SUM(B4:B6)</f>
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
+      <c r="B5" s="6">
+        <v>6</v>
+      </c>
+      <c r="C5" s="6">
+        <v>3</v>
       </c>
       <c r="D5" s="5">
         <f t="shared" ref="D5:D9" si="0">C5/B5</f>
@@ -1955,59 +1962,68 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
+        <v>46</v>
+      </c>
+      <c r="B6" s="6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="6">
+        <v>2</v>
       </c>
       <c r="D6" s="5">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="F6" s="5">
         <f>F5/F4</f>
         <v>0.6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D7" s="5" t="e">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="6">
+        <v>10</v>
+      </c>
+      <c r="C7" s="6">
+        <v>6</v>
+      </c>
+      <c r="D7" s="5">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>0.6</v>
       </c>
       <c r="F7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D8" s="5" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F8">
         <f>SUM(B7:B8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D9" s="5" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="F9">
         <f>SUM(C7:C8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="D10" s="5"/>
-      <c r="F10" s="5" t="e">
+      <c r="F10" s="5">
         <f>F9/F8</f>
-        <v>#DIV/0!</v>
+        <v>0.6</v>
       </c>
     </row>
   </sheetData>
@@ -2019,23 +2035,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2061,7 +2077,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>45277</v>
       </c>
@@ -2088,7 +2104,7 @@
         <v>70-80</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>45277</v>
       </c>
@@ -2115,7 +2131,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>45277</v>
       </c>
@@ -2142,7 +2158,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>45277</v>
       </c>
@@ -2169,7 +2185,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>45277</v>
       </c>
@@ -2196,7 +2212,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>45278</v>
       </c>
@@ -2214,13 +2230,16 @@
       </c>
       <c r="F7" t="s">
         <v>34</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
       </c>
       <c r="H7" t="str" cm="1">
         <f t="array" ref="H7">_xlfn.IFS(C7 &gt;= 0.85, "85  &lt;", AND(C7 &gt;=0.8, C7 &lt; 0.85), "80-85", AND(C7 &gt;= 0.7, C7 &lt; 0.8), "70-80", AND(C7 &gt;= 0.6, C7 &lt; 0.7),  "60-70", AND(C7 &gt;= 0.5, C7 &lt; 0.6), "50-60")</f>
         <v>70-80</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>45278</v>
       </c>
@@ -2238,13 +2257,16 @@
       </c>
       <c r="F8" t="s">
         <v>37</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
       </c>
       <c r="H8" t="str" cm="1">
         <f t="array" ref="H8">_xlfn.IFS(C8 &gt;= 0.85, "85  &lt;", AND(C8 &gt;=0.8, C8 &lt; 0.85), "80-85", AND(C8 &gt;= 0.7, C8 &lt; 0.8), "70-80", AND(C8 &gt;= 0.6, C8 &lt; 0.7),  "60-70", AND(C8 &gt;= 0.5, C8 &lt; 0.6), "50-60")</f>
         <v>60-70</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>45278</v>
       </c>
@@ -2262,13 +2284,16 @@
       </c>
       <c r="F9" t="s">
         <v>39</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
       </c>
       <c r="H9" t="str" cm="1">
         <f t="array" ref="H9">_xlfn.IFS(C9 &gt;= 0.85, "85  &lt;", AND(C9 &gt;=0.8, C9 &lt; 0.85), "80-85", AND(C9 &gt;= 0.7, C9 &lt; 0.8), "70-80", AND(C9 &gt;= 0.6, C9 &lt; 0.7),  "60-70", AND(C9 &gt;= 0.5, C9 &lt; 0.6), "50-60")</f>
         <v>60-70</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>45278</v>
       </c>
@@ -2286,13 +2311,16 @@
       </c>
       <c r="F10" t="s">
         <v>42</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
       </c>
       <c r="H10" t="str" cm="1">
         <f t="array" ref="H10">_xlfn.IFS(C10 &gt;= 0.85, "85  &lt;", AND(C10 &gt;=0.8, C10 &lt; 0.85), "80-85", AND(C10 &gt;= 0.7, C10 &lt; 0.8), "70-80", AND(C10 &gt;= 0.6, C10 &lt; 0.7),  "60-70", AND(C10 &gt;= 0.5, C10 &lt; 0.6), "50-60")</f>
         <v>50-60</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>45278</v>
       </c>
@@ -2310,313 +2338,316 @@
       </c>
       <c r="F11" t="s">
         <v>45</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
       </c>
       <c r="H11" t="str" cm="1">
         <f t="array" ref="H11">_xlfn.IFS(C11 &gt;= 0.85, "85  &lt;", AND(C11 &gt;=0.8, C11 &lt; 0.85), "80-85", AND(C11 &gt;= 0.7, C11 &lt; 0.8), "70-80", AND(C11 &gt;= 0.6, C11 &lt; 0.7),  "60-70", AND(C11 &gt;= 0.5, C11 &lt; 0.6), "50-60")</f>
         <v>50-60</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="C12" s="2"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="C13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="C14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="C15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="C16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="C17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="C18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="C19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="C20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="C21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="C22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="C23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="C24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="C25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="C26" s="2"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="C27" s="2"/>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="C28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="C29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="C30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="C31" s="2"/>
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
       <c r="C32" s="2"/>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
       <c r="C33" s="2"/>
       <c r="E33" s="2"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
       <c r="C34" s="2"/>
       <c r="E34" s="2"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
       <c r="C35" s="2"/>
       <c r="E35" s="2"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
       <c r="C36" s="2"/>
       <c r="E36" s="2"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
       <c r="C37" s="2"/>
       <c r="E37" s="2"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
       <c r="C38" s="2"/>
       <c r="E38" s="2"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
       <c r="C39" s="2"/>
       <c r="E39" s="2"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
       <c r="C40" s="2"/>
       <c r="E40" s="2"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="1"/>
       <c r="C41" s="2"/>
       <c r="E41" s="2"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="1"/>
       <c r="C42" s="2"/>
       <c r="E42" s="2"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="1"/>
       <c r="C43" s="2"/>
       <c r="E43" s="2"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="1"/>
       <c r="C44" s="2"/>
       <c r="E44" s="2"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="1"/>
       <c r="C45" s="2"/>
       <c r="E45" s="2"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="1"/>
       <c r="C46" s="2"/>
       <c r="E46" s="2"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="1"/>
       <c r="C47" s="2"/>
       <c r="E47" s="2"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="1"/>
       <c r="C48" s="2"/>
       <c r="E48" s="2"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="1"/>
       <c r="C49" s="2"/>
       <c r="E49" s="2"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="1"/>
       <c r="C50" s="2"/>
       <c r="E50" s="2"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="1"/>
       <c r="C51" s="2"/>
       <c r="E51" s="2"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="1"/>
       <c r="C52" s="2"/>
       <c r="E52" s="2"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="1"/>
       <c r="C53" s="2"/>
       <c r="E53" s="2"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="1"/>
       <c r="C54" s="2"/>
       <c r="E54" s="2"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="1"/>
       <c r="C55" s="2"/>
       <c r="E55" s="2"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="1"/>
       <c r="C56" s="2"/>
       <c r="E56" s="2"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="1"/>
       <c r="C57" s="2"/>
       <c r="E57" s="2"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="1"/>
       <c r="C58" s="2"/>
       <c r="E58" s="2"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="1"/>
       <c r="C59" s="2"/>
       <c r="E59" s="2"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="1"/>
       <c r="C60" s="2"/>
       <c r="E60" s="2"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="1"/>
       <c r="C61" s="2"/>
       <c r="E61" s="2"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="1"/>
       <c r="C62" s="2"/>
       <c r="E62" s="2"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="1"/>
       <c r="C63" s="2"/>
       <c r="E63" s="2"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="1"/>
       <c r="C64" s="2"/>
       <c r="E64" s="2"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="1"/>
       <c r="C65" s="2"/>
       <c r="E65" s="2"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="1"/>
       <c r="C66" s="2"/>
       <c r="E66" s="2"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="1"/>
       <c r="C67" s="2"/>
       <c r="E67" s="2"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="1"/>
       <c r="C68" s="2"/>
       <c r="E68" s="2"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="1"/>
       <c r="C69" s="2"/>
       <c r="E69" s="2"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="1"/>
       <c r="C70" s="2"/>
       <c r="E70" s="2"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="1"/>
       <c r="C71" s="2"/>
       <c r="E71" s="2"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="1"/>
       <c r="C72" s="2"/>
       <c r="E72" s="2"/>

</xml_diff>

<commit_message>
updated models and predictions
</commit_message>
<xml_diff>
--- a/ANN Lifetime Predictions.xlsx
+++ b/ANN Lifetime Predictions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thigg\Desktop\Hockey Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E6BC553-56D2-4D1A-99D5-7DB330BBEA1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B168CC-D4A0-44C6-A127-99F8FE13BFBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1740" yWindow="1185" windowWidth="19125" windowHeight="11235" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pivot" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId3"/>
+    <pivotCache cacheId="5" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="68">
   <si>
     <t>Date</t>
   </si>
@@ -200,6 +200,69 @@
   </si>
   <si>
     <t>50-60</t>
+  </si>
+  <si>
+    <t>Tampa Bay Lightning</t>
+  </si>
+  <si>
+    <t>St. Louis Blues</t>
+  </si>
+  <si>
+    <t>Playing At:  Tampa Bay Lightning   Home</t>
+  </si>
+  <si>
+    <t>Boston Bruins</t>
+  </si>
+  <si>
+    <t>Playing At:  Boston Bruins   Home</t>
+  </si>
+  <si>
+    <t>Los Angeles Kings</t>
+  </si>
+  <si>
+    <t>Playing At:  San Jose Sharks   Home</t>
+  </si>
+  <si>
+    <t>Buffalo Sabres</t>
+  </si>
+  <si>
+    <t>Columbus Blue Jackets</t>
+  </si>
+  <si>
+    <t>Playing At:  Buffalo Sabres   Home</t>
+  </si>
+  <si>
+    <t>Philadelphia Flyers</t>
+  </si>
+  <si>
+    <t>Edmonton Oilers</t>
+  </si>
+  <si>
+    <t>New York Islanders</t>
+  </si>
+  <si>
+    <t>Playing At:  New York Islanders   Home</t>
+  </si>
+  <si>
+    <t>Arizona Coyotes</t>
+  </si>
+  <si>
+    <t>Playing At:  Arizona Coyotes   Home</t>
+  </si>
+  <si>
+    <t>Nashville Predators</t>
+  </si>
+  <si>
+    <t>Playing At:  Nashville Predators   Home</t>
+  </si>
+  <si>
+    <t>Toronto Maple Leafs</t>
+  </si>
+  <si>
+    <t>New York Rangers</t>
+  </si>
+  <si>
+    <t>Playing At:  Toronto Maple Leafs   Home</t>
   </si>
 </sst>
 </file>
@@ -684,7 +747,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -693,7 +756,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1527,7 +1589,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C7" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField showAll="0"/>
@@ -1894,20 +1956,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -1924,14 +1986,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" s="5">
@@ -1943,14 +2005,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5">
         <v>6</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5">
         <v>3</v>
       </c>
       <c r="D5" s="5">
@@ -1962,14 +2024,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6">
         <v>2</v>
       </c>
       <c r="D6" s="5">
@@ -1981,14 +2043,14 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7">
         <v>10</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7">
         <v>6</v>
       </c>
       <c r="D7" s="5">
@@ -1999,7 +2061,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D8" s="5" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2009,7 +2071,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D9" s="5" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2019,7 +2081,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D10" s="5"/>
       <c r="F10" s="5">
         <f>F9/F8</f>
@@ -2035,23 +2097,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2077,7 +2139,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45277</v>
       </c>
@@ -2104,7 +2166,7 @@
         <v>70-80</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45277</v>
       </c>
@@ -2131,7 +2193,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45277</v>
       </c>
@@ -2158,7 +2220,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45277</v>
       </c>
@@ -2185,7 +2247,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45277</v>
       </c>
@@ -2212,7 +2274,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45278</v>
       </c>
@@ -2239,7 +2301,7 @@
         <v>70-80</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45278</v>
       </c>
@@ -2266,7 +2328,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45278</v>
       </c>
@@ -2293,7 +2355,7 @@
         <v>60-70</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45278</v>
       </c>
@@ -2320,7 +2382,7 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45278</v>
       </c>
@@ -2347,307 +2409,516 @@
         <v>50-60</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
-      <c r="C12" s="2"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
-      <c r="C13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="1"/>
-      <c r="C14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="1"/>
-      <c r="C15" s="2"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="1"/>
-      <c r="C16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="1"/>
-      <c r="C17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="1"/>
-      <c r="C18" s="2"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="1"/>
-      <c r="C19" s="2"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="1"/>
-      <c r="C20" s="2"/>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="1"/>
-      <c r="C21" s="2"/>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="1"/>
-      <c r="C22" s="2"/>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>45279</v>
+      </c>
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.81533999999999995</v>
+      </c>
+      <c r="D12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.18465999999999999</v>
+      </c>
+      <c r="F12" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" t="str" cm="1">
+        <f t="array" ref="H12">_xlfn.IFS(C12 &gt;= 0.85, "85  &lt;", AND(C12 &gt;=0.8, C12 &lt; 0.85), "80-85", AND(C12 &gt;= 0.7, C12 &lt; 0.8), "70-80", AND(C12 &gt;= 0.6, C12 &lt; 0.7),  "60-70", AND(C12 &gt;= 0.5, C12 &lt; 0.6), "50-60")</f>
+        <v>80-85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>45279</v>
+      </c>
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.76312000000000002</v>
+      </c>
+      <c r="D13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.23688000000000001</v>
+      </c>
+      <c r="F13" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" t="str" cm="1">
+        <f t="array" ref="H13">_xlfn.IFS(C13 &gt;= 0.85, "85  &lt;", AND(C13 &gt;=0.8, C13 &lt; 0.85), "80-85", AND(C13 &gt;= 0.7, C13 &lt; 0.8), "70-80", AND(C13 &gt;= 0.6, C13 &lt; 0.7),  "60-70", AND(C13 &gt;= 0.5, C13 &lt; 0.6), "50-60")</f>
+        <v>70-80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>45279</v>
+      </c>
+      <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.76288999999999996</v>
+      </c>
+      <c r="D14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.23710999999999999</v>
+      </c>
+      <c r="F14" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" t="str" cm="1">
+        <f t="array" ref="H14">_xlfn.IFS(C14 &gt;= 0.85, "85  &lt;", AND(C14 &gt;=0.8, C14 &lt; 0.85), "80-85", AND(C14 &gt;= 0.7, C14 &lt; 0.8), "70-80", AND(C14 &gt;= 0.6, C14 &lt; 0.7),  "60-70", AND(C14 &gt;= 0.5, C14 &lt; 0.6), "50-60")</f>
+        <v>70-80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>45279</v>
+      </c>
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.72492999999999996</v>
+      </c>
+      <c r="D15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.27506999999999998</v>
+      </c>
+      <c r="F15" t="s">
+        <v>56</v>
+      </c>
+      <c r="H15" t="str" cm="1">
+        <f t="array" ref="H15">_xlfn.IFS(C15 &gt;= 0.85, "85  &lt;", AND(C15 &gt;=0.8, C15 &lt; 0.85), "80-85", AND(C15 &gt;= 0.7, C15 &lt; 0.8), "70-80", AND(C15 &gt;= 0.6, C15 &lt; 0.7),  "60-70", AND(C15 &gt;= 0.5, C15 &lt; 0.6), "50-60")</f>
+        <v>70-80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>45279</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.68744000000000005</v>
+      </c>
+      <c r="D16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.31256</v>
+      </c>
+      <c r="F16" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16" t="str" cm="1">
+        <f t="array" ref="H16">_xlfn.IFS(C16 &gt;= 0.85, "85  &lt;", AND(C16 &gt;=0.8, C16 &lt; 0.85), "80-85", AND(C16 &gt;= 0.7, C16 &lt; 0.8), "70-80", AND(C16 &gt;= 0.6, C16 &lt; 0.7),  "60-70", AND(C16 &gt;= 0.5, C16 &lt; 0.6), "50-60")</f>
+        <v>60-70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>45279</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.67522000000000004</v>
+      </c>
+      <c r="D17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.32478000000000001</v>
+      </c>
+      <c r="F17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H17" t="str" cm="1">
+        <f t="array" ref="H17">_xlfn.IFS(C17 &gt;= 0.85, "85  &lt;", AND(C17 &gt;=0.8, C17 &lt; 0.85), "80-85", AND(C17 &gt;= 0.7, C17 &lt; 0.8), "70-80", AND(C17 &gt;= 0.6, C17 &lt; 0.7),  "60-70", AND(C17 &gt;= 0.5, C17 &lt; 0.6), "50-60")</f>
+        <v>60-70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>45279</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.67174999999999996</v>
+      </c>
+      <c r="D18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.32824999999999999</v>
+      </c>
+      <c r="F18" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" t="str" cm="1">
+        <f t="array" ref="H18">_xlfn.IFS(C18 &gt;= 0.85, "85  &lt;", AND(C18 &gt;=0.8, C18 &lt; 0.85), "80-85", AND(C18 &gt;= 0.7, C18 &lt; 0.8), "70-80", AND(C18 &gt;= 0.6, C18 &lt; 0.7),  "60-70", AND(C18 &gt;= 0.5, C18 &lt; 0.6), "50-60")</f>
+        <v>60-70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>45279</v>
+      </c>
+      <c r="B19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.64061000000000001</v>
+      </c>
+      <c r="D19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.35938999999999999</v>
+      </c>
+      <c r="F19" t="s">
+        <v>60</v>
+      </c>
+      <c r="H19" t="str" cm="1">
+        <f t="array" ref="H19">_xlfn.IFS(C19 &gt;= 0.85, "85  &lt;", AND(C19 &gt;=0.8, C19 &lt; 0.85), "80-85", AND(C19 &gt;= 0.7, C19 &lt; 0.8), "70-80", AND(C19 &gt;= 0.6, C19 &lt; 0.7),  "60-70", AND(C19 &gt;= 0.5, C19 &lt; 0.6), "50-60")</f>
+        <v>60-70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>45279</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.58294999999999997</v>
+      </c>
+      <c r="D20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.41704999999999998</v>
+      </c>
+      <c r="F20" t="s">
+        <v>62</v>
+      </c>
+      <c r="H20" t="str" cm="1">
+        <f t="array" ref="H20">_xlfn.IFS(C20 &gt;= 0.85, "85  &lt;", AND(C20 &gt;=0.8, C20 &lt; 0.85), "80-85", AND(C20 &gt;= 0.7, C20 &lt; 0.8), "70-80", AND(C20 &gt;= 0.6, C20 &lt; 0.7),  "60-70", AND(C20 &gt;= 0.5, C20 &lt; 0.6), "50-60")</f>
+        <v>50-60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>45279</v>
+      </c>
+      <c r="B21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.58067000000000002</v>
+      </c>
+      <c r="D21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.41932999999999998</v>
+      </c>
+      <c r="F21" t="s">
+        <v>64</v>
+      </c>
+      <c r="H21" t="str" cm="1">
+        <f t="array" ref="H21">_xlfn.IFS(C21 &gt;= 0.85, "85  &lt;", AND(C21 &gt;=0.8, C21 &lt; 0.85), "80-85", AND(C21 &gt;= 0.7, C21 &lt; 0.8), "70-80", AND(C21 &gt;= 0.6, C21 &lt; 0.7),  "60-70", AND(C21 &gt;= 0.5, C21 &lt; 0.6), "50-60")</f>
+        <v>50-60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>45279</v>
+      </c>
+      <c r="B22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.52131000000000005</v>
+      </c>
+      <c r="D22" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.47869</v>
+      </c>
+      <c r="F22" t="s">
+        <v>67</v>
+      </c>
+      <c r="H22" t="str" cm="1">
+        <f t="array" ref="H22">_xlfn.IFS(C22 &gt;= 0.85, "85  &lt;", AND(C22 &gt;=0.8, C22 &lt; 0.85), "80-85", AND(C22 &gt;= 0.7, C22 &lt; 0.8), "70-80", AND(C22 &gt;= 0.6, C22 &lt; 0.7),  "60-70", AND(C22 &gt;= 0.5, C22 &lt; 0.6), "50-60")</f>
+        <v>50-60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="C23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="C24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="C25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="C26" s="2"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="C27" s="2"/>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="C28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="C29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="C30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="C31" s="2"/>
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="C32" s="2"/>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="C33" s="2"/>
       <c r="E33" s="2"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="C34" s="2"/>
       <c r="E34" s="2"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="C35" s="2"/>
       <c r="E35" s="2"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="C36" s="2"/>
       <c r="E36" s="2"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="C37" s="2"/>
       <c r="E37" s="2"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="C38" s="2"/>
       <c r="E38" s="2"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="C39" s="2"/>
       <c r="E39" s="2"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="C40" s="2"/>
       <c r="E40" s="2"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="C41" s="2"/>
       <c r="E41" s="2"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="C42" s="2"/>
       <c r="E42" s="2"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="C43" s="2"/>
       <c r="E43" s="2"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="C44" s="2"/>
       <c r="E44" s="2"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="C45" s="2"/>
       <c r="E45" s="2"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="C46" s="2"/>
       <c r="E46" s="2"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="C47" s="2"/>
       <c r="E47" s="2"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="C48" s="2"/>
       <c r="E48" s="2"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="C49" s="2"/>
       <c r="E49" s="2"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="C50" s="2"/>
       <c r="E50" s="2"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="C51" s="2"/>
       <c r="E51" s="2"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="C52" s="2"/>
       <c r="E52" s="2"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="C53" s="2"/>
       <c r="E53" s="2"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="C54" s="2"/>
       <c r="E54" s="2"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="C55" s="2"/>
       <c r="E55" s="2"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="C56" s="2"/>
       <c r="E56" s="2"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="C57" s="2"/>
       <c r="E57" s="2"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="C58" s="2"/>
       <c r="E58" s="2"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="C59" s="2"/>
       <c r="E59" s="2"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="C60" s="2"/>
       <c r="E60" s="2"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="C61" s="2"/>
       <c r="E61" s="2"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="C62" s="2"/>
       <c r="E62" s="2"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="C63" s="2"/>
       <c r="E63" s="2"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="C64" s="2"/>
       <c r="E64" s="2"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="C65" s="2"/>
       <c r="E65" s="2"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="C66" s="2"/>
       <c r="E66" s="2"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="C67" s="2"/>
       <c r="E67" s="2"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="C68" s="2"/>
       <c r="E68" s="2"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="C69" s="2"/>
       <c r="E69" s="2"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="C70" s="2"/>
       <c r="E70" s="2"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="C71" s="2"/>
       <c r="E71" s="2"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="C72" s="2"/>
       <c r="E72" s="2"/>

</xml_diff>